<commit_message>
updated  font size and experiment
</commit_message>
<xml_diff>
--- a/Study/conditions.xlsx
+++ b/Study/conditions.xlsx
@@ -1182,64 +1182,64 @@
         <v>21</v>
       </c>
       <c r="B2">
-        <v>434</v>
+        <v>593</v>
       </c>
       <c r="C2">
-        <v>181</v>
+        <v>235</v>
       </c>
       <c r="D2" t="s">
         <v>53</v>
       </c>
       <c r="E2">
-        <v>362</v>
+        <v>494</v>
       </c>
       <c r="F2">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="G2" t="s">
         <v>85</v>
       </c>
       <c r="H2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I2">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J2" t="s">
         <v>117</v>
       </c>
       <c r="K2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L2">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M2" t="s">
         <v>149</v>
       </c>
       <c r="N2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O2">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P2" t="s">
         <v>181</v>
       </c>
       <c r="Q2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R2">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S2" t="s">
         <v>213</v>
       </c>
       <c r="T2">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U2">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -1247,64 +1247,64 @@
         <v>22</v>
       </c>
       <c r="B3">
-        <v>418</v>
+        <v>571</v>
       </c>
       <c r="C3">
-        <v>238</v>
+        <v>310</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>
       </c>
       <c r="E3">
-        <v>394</v>
+        <v>538</v>
       </c>
       <c r="F3">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="G3" t="s">
         <v>86</v>
       </c>
       <c r="H3">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="I3">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J3" t="s">
         <v>118</v>
       </c>
       <c r="K3">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="L3">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M3" t="s">
         <v>150</v>
       </c>
       <c r="N3">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="O3">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P3" t="s">
         <v>182</v>
       </c>
       <c r="Q3">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R3">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S3" t="s">
         <v>214</v>
       </c>
       <c r="T3">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U3">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -1312,64 +1312,64 @@
         <v>23</v>
       </c>
       <c r="B4">
-        <v>658</v>
+        <v>901</v>
       </c>
       <c r="C4">
-        <v>295</v>
+        <v>385</v>
       </c>
       <c r="D4" t="s">
         <v>55</v>
       </c>
       <c r="E4">
-        <v>650</v>
+        <v>890</v>
       </c>
       <c r="F4">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="G4" t="s">
         <v>87</v>
       </c>
       <c r="H4">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I4">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J4" t="s">
         <v>119</v>
       </c>
       <c r="K4">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L4">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M4" t="s">
         <v>151</v>
       </c>
       <c r="N4">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="O4">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P4" t="s">
         <v>183</v>
       </c>
       <c r="Q4">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R4">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S4" t="s">
         <v>215</v>
       </c>
       <c r="T4">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U4">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -1377,64 +1377,64 @@
         <v>24</v>
       </c>
       <c r="B5">
-        <v>466</v>
+        <v>637</v>
       </c>
       <c r="C5">
-        <v>238</v>
+        <v>310</v>
       </c>
       <c r="D5" t="s">
         <v>56</v>
       </c>
       <c r="E5">
-        <v>426</v>
+        <v>582</v>
       </c>
       <c r="F5">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="G5" t="s">
         <v>88</v>
       </c>
       <c r="H5">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I5">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J5" t="s">
         <v>120</v>
       </c>
       <c r="K5">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L5">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M5" t="s">
         <v>152</v>
       </c>
       <c r="N5">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O5">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P5" t="s">
         <v>184</v>
       </c>
       <c r="Q5">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R5">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S5" t="s">
         <v>216</v>
       </c>
       <c r="T5">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U5">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -1442,64 +1442,64 @@
         <v>25</v>
       </c>
       <c r="B6">
-        <v>474</v>
+        <v>648</v>
       </c>
       <c r="C6">
-        <v>181</v>
+        <v>235</v>
       </c>
       <c r="D6" t="s">
         <v>57</v>
       </c>
       <c r="E6">
-        <v>538</v>
+        <v>736</v>
       </c>
       <c r="F6">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="G6" t="s">
         <v>89</v>
       </c>
       <c r="H6">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I6">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J6" t="s">
         <v>121</v>
       </c>
       <c r="K6">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L6">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M6" t="s">
         <v>153</v>
       </c>
       <c r="N6">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O6">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P6" t="s">
         <v>185</v>
       </c>
       <c r="Q6">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R6">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S6" t="s">
         <v>217</v>
       </c>
       <c r="T6">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U6">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -1507,64 +1507,64 @@
         <v>26</v>
       </c>
       <c r="B7">
-        <v>426</v>
+        <v>582</v>
       </c>
       <c r="C7">
-        <v>447</v>
+        <v>585</v>
       </c>
       <c r="D7" t="s">
         <v>58</v>
       </c>
       <c r="E7">
-        <v>362</v>
+        <v>494</v>
       </c>
       <c r="F7">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="G7" t="s">
         <v>90</v>
       </c>
       <c r="H7">
-        <v>130</v>
+        <v>175</v>
       </c>
       <c r="I7">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J7" t="s">
         <v>122</v>
       </c>
       <c r="K7">
-        <v>130</v>
+        <v>175</v>
       </c>
       <c r="L7">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M7" t="s">
         <v>154</v>
       </c>
       <c r="N7">
-        <v>130</v>
+        <v>175</v>
       </c>
       <c r="O7">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P7" t="s">
         <v>186</v>
       </c>
       <c r="Q7">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R7">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S7" t="s">
         <v>218</v>
       </c>
       <c r="T7">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U7">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -1572,64 +1572,64 @@
         <v>27</v>
       </c>
       <c r="B8">
-        <v>578</v>
+        <v>791</v>
       </c>
       <c r="C8">
-        <v>219</v>
+        <v>285</v>
       </c>
       <c r="D8" t="s">
         <v>59</v>
       </c>
       <c r="E8">
-        <v>378</v>
+        <v>516</v>
       </c>
       <c r="F8">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="G8" t="s">
         <v>91</v>
       </c>
       <c r="H8">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I8">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J8" t="s">
         <v>123</v>
       </c>
       <c r="K8">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="L8">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M8" t="s">
         <v>155</v>
       </c>
       <c r="N8">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="O8">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P8" t="s">
         <v>187</v>
       </c>
       <c r="Q8">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R8">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S8" t="s">
         <v>219</v>
       </c>
       <c r="T8">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U8">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1637,64 +1637,64 @@
         <v>28</v>
       </c>
       <c r="B9">
-        <v>618</v>
+        <v>846</v>
       </c>
       <c r="C9">
-        <v>409</v>
+        <v>535</v>
       </c>
       <c r="D9" t="s">
         <v>60</v>
       </c>
       <c r="E9">
-        <v>514</v>
+        <v>703</v>
       </c>
       <c r="F9">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="G9" t="s">
         <v>92</v>
       </c>
       <c r="H9">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="I9">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J9" t="s">
         <v>124</v>
       </c>
       <c r="K9">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="L9">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M9" t="s">
         <v>156</v>
       </c>
       <c r="N9">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O9">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P9" t="s">
         <v>188</v>
       </c>
       <c r="Q9">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R9">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S9" t="s">
         <v>220</v>
       </c>
       <c r="T9">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U9">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -1702,64 +1702,64 @@
         <v>29</v>
       </c>
       <c r="B10">
-        <v>450</v>
+        <v>615</v>
       </c>
       <c r="C10">
-        <v>333</v>
+        <v>435</v>
       </c>
       <c r="D10" t="s">
         <v>61</v>
       </c>
       <c r="E10">
-        <v>386</v>
+        <v>527</v>
       </c>
       <c r="F10">
-        <v>257</v>
+        <v>335</v>
       </c>
       <c r="G10" t="s">
         <v>93</v>
       </c>
       <c r="H10">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="I10">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J10" t="s">
         <v>125</v>
       </c>
       <c r="K10">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="L10">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M10" t="s">
         <v>157</v>
       </c>
       <c r="N10">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="O10">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P10" t="s">
         <v>189</v>
       </c>
       <c r="Q10">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R10">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S10" t="s">
         <v>221</v>
       </c>
       <c r="T10">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U10">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1767,64 +1767,64 @@
         <v>30</v>
       </c>
       <c r="B11">
-        <v>538</v>
+        <v>736</v>
       </c>
       <c r="C11">
-        <v>561</v>
+        <v>735</v>
       </c>
       <c r="D11" t="s">
         <v>62</v>
       </c>
       <c r="E11">
-        <v>370</v>
+        <v>505</v>
       </c>
       <c r="F11">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="G11" t="s">
         <v>94</v>
       </c>
       <c r="H11">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="I11">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J11" t="s">
         <v>126</v>
       </c>
       <c r="K11">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="L11">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M11" t="s">
         <v>158</v>
       </c>
       <c r="N11">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="O11">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P11" t="s">
         <v>190</v>
       </c>
       <c r="Q11">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R11">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S11" t="s">
         <v>222</v>
       </c>
       <c r="T11">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U11">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1832,64 +1832,64 @@
         <v>31</v>
       </c>
       <c r="B12">
-        <v>578</v>
+        <v>791</v>
       </c>
       <c r="C12">
-        <v>352</v>
+        <v>460</v>
       </c>
       <c r="D12" t="s">
         <v>63</v>
       </c>
       <c r="E12">
-        <v>554</v>
+        <v>758</v>
       </c>
       <c r="F12">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="G12" t="s">
         <v>95</v>
       </c>
       <c r="H12">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I12">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J12" t="s">
         <v>127</v>
       </c>
       <c r="K12">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="L12">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M12" t="s">
         <v>159</v>
       </c>
       <c r="N12">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="O12">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P12" t="s">
         <v>191</v>
       </c>
       <c r="Q12">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R12">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S12" t="s">
         <v>223</v>
       </c>
       <c r="T12">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U12">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1897,64 +1897,64 @@
         <v>32</v>
       </c>
       <c r="B13">
-        <v>642</v>
+        <v>879</v>
       </c>
       <c r="C13">
-        <v>333</v>
+        <v>435</v>
       </c>
       <c r="D13" t="s">
         <v>64</v>
       </c>
       <c r="E13">
-        <v>386</v>
+        <v>527</v>
       </c>
       <c r="F13">
-        <v>181</v>
+        <v>235</v>
       </c>
       <c r="G13" t="s">
         <v>96</v>
       </c>
       <c r="H13">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I13">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J13" t="s">
         <v>128</v>
       </c>
       <c r="K13">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L13">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M13" t="s">
         <v>160</v>
       </c>
       <c r="N13">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O13">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P13" t="s">
         <v>192</v>
       </c>
       <c r="Q13">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R13">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S13" t="s">
         <v>224</v>
       </c>
       <c r="T13">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U13">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1962,64 +1962,64 @@
         <v>33</v>
       </c>
       <c r="B14">
-        <v>378</v>
+        <v>516</v>
       </c>
       <c r="C14">
-        <v>295</v>
+        <v>385</v>
       </c>
       <c r="D14" t="s">
         <v>65</v>
       </c>
       <c r="E14">
-        <v>362</v>
+        <v>494</v>
       </c>
       <c r="F14">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="G14" t="s">
         <v>97</v>
       </c>
       <c r="H14">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I14">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J14" t="s">
         <v>129</v>
       </c>
       <c r="K14">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L14">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M14" t="s">
         <v>161</v>
       </c>
       <c r="N14">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O14">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P14" t="s">
         <v>193</v>
       </c>
       <c r="Q14">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R14">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S14" t="s">
         <v>225</v>
       </c>
       <c r="T14">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="U14">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -2027,64 +2027,64 @@
         <v>34</v>
       </c>
       <c r="B15">
-        <v>426</v>
+        <v>582</v>
       </c>
       <c r="C15">
-        <v>295</v>
+        <v>385</v>
       </c>
       <c r="D15" t="s">
         <v>66</v>
       </c>
       <c r="E15">
-        <v>354</v>
+        <v>483</v>
       </c>
       <c r="F15">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="G15" t="s">
         <v>98</v>
       </c>
       <c r="H15">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="I15">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J15" t="s">
         <v>130</v>
       </c>
       <c r="K15">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="L15">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M15" t="s">
         <v>162</v>
       </c>
       <c r="N15">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="O15">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P15" t="s">
         <v>194</v>
       </c>
       <c r="Q15">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R15">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S15" t="s">
         <v>226</v>
       </c>
       <c r="T15">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U15">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -2092,64 +2092,64 @@
         <v>35</v>
       </c>
       <c r="B16">
-        <v>530</v>
+        <v>725</v>
       </c>
       <c r="C16">
-        <v>542</v>
+        <v>710</v>
       </c>
       <c r="D16" t="s">
         <v>67</v>
       </c>
       <c r="E16">
-        <v>442</v>
+        <v>604</v>
       </c>
       <c r="F16">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="G16" t="s">
         <v>99</v>
       </c>
       <c r="H16">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="I16">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J16" t="s">
         <v>131</v>
       </c>
       <c r="K16">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="L16">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M16" t="s">
         <v>163</v>
       </c>
       <c r="N16">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="O16">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P16" t="s">
         <v>195</v>
       </c>
       <c r="Q16">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R16">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S16" t="s">
         <v>227</v>
       </c>
       <c r="T16">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U16">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -2157,64 +2157,64 @@
         <v>36</v>
       </c>
       <c r="B17">
-        <v>386</v>
+        <v>527</v>
       </c>
       <c r="C17">
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="D17" t="s">
         <v>68</v>
       </c>
       <c r="E17">
-        <v>346</v>
+        <v>472</v>
       </c>
       <c r="F17">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="G17" t="s">
         <v>100</v>
       </c>
       <c r="H17">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="I17">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J17" t="s">
         <v>132</v>
       </c>
       <c r="K17">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="L17">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M17" t="s">
         <v>164</v>
       </c>
       <c r="N17">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O17">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P17" t="s">
         <v>196</v>
       </c>
       <c r="Q17">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R17">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S17" t="s">
         <v>228</v>
       </c>
       <c r="T17">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U17">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -2222,64 +2222,64 @@
         <v>37</v>
       </c>
       <c r="B18">
-        <v>546</v>
+        <v>747</v>
       </c>
       <c r="C18">
-        <v>333</v>
+        <v>435</v>
       </c>
       <c r="D18" t="s">
         <v>69</v>
       </c>
       <c r="E18">
-        <v>418</v>
+        <v>571</v>
       </c>
       <c r="F18">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="G18" t="s">
         <v>101</v>
       </c>
       <c r="H18">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I18">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J18" t="s">
         <v>133</v>
       </c>
       <c r="K18">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="L18">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M18" t="s">
         <v>165</v>
       </c>
       <c r="N18">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O18">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P18" t="s">
         <v>197</v>
       </c>
       <c r="Q18">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R18">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S18" t="s">
         <v>229</v>
       </c>
       <c r="T18">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U18">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -2287,64 +2287,64 @@
         <v>38</v>
       </c>
       <c r="B19">
-        <v>354</v>
+        <v>483</v>
       </c>
       <c r="C19">
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="D19" t="s">
         <v>70</v>
       </c>
       <c r="E19">
-        <v>346</v>
+        <v>472</v>
       </c>
       <c r="F19">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="G19" t="s">
         <v>102</v>
       </c>
       <c r="H19">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="I19">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J19" t="s">
         <v>134</v>
       </c>
       <c r="K19">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L19">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M19" t="s">
         <v>166</v>
       </c>
       <c r="N19">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O19">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P19" t="s">
         <v>198</v>
       </c>
       <c r="Q19">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R19">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S19" t="s">
         <v>230</v>
       </c>
       <c r="T19">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U19">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -2352,64 +2352,64 @@
         <v>39</v>
       </c>
       <c r="B20">
-        <v>578</v>
+        <v>791</v>
       </c>
       <c r="C20">
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="D20" t="s">
         <v>71</v>
       </c>
       <c r="E20">
-        <v>402</v>
+        <v>549</v>
       </c>
       <c r="F20">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="G20" t="s">
         <v>103</v>
       </c>
       <c r="H20">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="I20">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J20" t="s">
         <v>135</v>
       </c>
       <c r="K20">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="L20">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M20" t="s">
         <v>167</v>
       </c>
       <c r="N20">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="O20">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P20" t="s">
         <v>199</v>
       </c>
       <c r="Q20">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R20">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S20" t="s">
         <v>231</v>
       </c>
       <c r="T20">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U20">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -2417,64 +2417,64 @@
         <v>40</v>
       </c>
       <c r="B21">
-        <v>538</v>
+        <v>736</v>
       </c>
       <c r="C21">
-        <v>447</v>
+        <v>585</v>
       </c>
       <c r="D21" t="s">
         <v>72</v>
       </c>
       <c r="E21">
-        <v>402</v>
+        <v>549</v>
       </c>
       <c r="F21">
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="G21" t="s">
         <v>104</v>
       </c>
       <c r="H21">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="I21">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="J21" t="s">
         <v>136</v>
       </c>
       <c r="K21">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L21">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M21" t="s">
         <v>168</v>
       </c>
       <c r="N21">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="O21">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P21" t="s">
         <v>200</v>
       </c>
       <c r="Q21">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R21">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S21" t="s">
         <v>232</v>
       </c>
       <c r="T21">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U21">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -2482,64 +2482,64 @@
         <v>41</v>
       </c>
       <c r="B22">
-        <v>434</v>
+        <v>593</v>
       </c>
       <c r="C22">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="D22" t="s">
         <v>73</v>
       </c>
       <c r="E22">
-        <v>346</v>
+        <v>472</v>
       </c>
       <c r="F22">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="G22" t="s">
         <v>105</v>
       </c>
       <c r="H22">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I22">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J22" t="s">
         <v>137</v>
       </c>
       <c r="K22">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="L22">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M22" t="s">
         <v>169</v>
       </c>
       <c r="N22">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="O22">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P22" t="s">
         <v>201</v>
       </c>
       <c r="Q22">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R22">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S22" t="s">
         <v>233</v>
       </c>
       <c r="T22">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U22">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -2547,64 +2547,64 @@
         <v>42</v>
       </c>
       <c r="B23">
-        <v>458</v>
+        <v>626</v>
       </c>
       <c r="C23">
-        <v>314</v>
+        <v>410</v>
       </c>
       <c r="D23" t="s">
         <v>74</v>
       </c>
       <c r="E23">
-        <v>410</v>
+        <v>560</v>
       </c>
       <c r="F23">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="G23" t="s">
         <v>106</v>
       </c>
       <c r="H23">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I23">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J23" t="s">
         <v>138</v>
       </c>
       <c r="K23">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L23">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M23" t="s">
         <v>170</v>
       </c>
       <c r="N23">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O23">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P23" t="s">
         <v>202</v>
       </c>
       <c r="Q23">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R23">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S23" t="s">
         <v>234</v>
       </c>
       <c r="T23">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U23">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -2612,64 +2612,64 @@
         <v>43</v>
       </c>
       <c r="B24">
-        <v>442</v>
+        <v>604</v>
       </c>
       <c r="C24">
-        <v>504</v>
+        <v>660</v>
       </c>
       <c r="D24" t="s">
         <v>75</v>
       </c>
       <c r="E24">
-        <v>442</v>
+        <v>604</v>
       </c>
       <c r="F24">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="G24" t="s">
         <v>107</v>
       </c>
       <c r="H24">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="I24">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="J24" t="s">
         <v>139</v>
       </c>
       <c r="K24">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="L24">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M24" t="s">
         <v>171</v>
       </c>
       <c r="N24">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="O24">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P24" t="s">
         <v>203</v>
       </c>
       <c r="Q24">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R24">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S24" t="s">
         <v>235</v>
       </c>
       <c r="T24">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U24">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -2677,64 +2677,64 @@
         <v>44</v>
       </c>
       <c r="B25">
-        <v>434</v>
+        <v>593</v>
       </c>
       <c r="C25">
-        <v>219</v>
+        <v>285</v>
       </c>
       <c r="D25" t="s">
         <v>76</v>
       </c>
       <c r="E25">
-        <v>346</v>
+        <v>472</v>
       </c>
       <c r="F25">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="G25" t="s">
         <v>108</v>
       </c>
       <c r="H25">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I25">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J25" t="s">
         <v>140</v>
       </c>
       <c r="K25">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="L25">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M25" t="s">
         <v>172</v>
       </c>
       <c r="N25">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="O25">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P25" t="s">
         <v>204</v>
       </c>
       <c r="Q25">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R25">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S25" t="s">
         <v>236</v>
       </c>
       <c r="T25">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U25">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -2742,64 +2742,64 @@
         <v>45</v>
       </c>
       <c r="B26">
-        <v>498</v>
+        <v>681</v>
       </c>
       <c r="C26">
-        <v>371</v>
+        <v>485</v>
       </c>
       <c r="D26" t="s">
         <v>77</v>
       </c>
       <c r="E26">
-        <v>442</v>
+        <v>604</v>
       </c>
       <c r="F26">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="G26" t="s">
         <v>109</v>
       </c>
       <c r="H26">
-        <v>138</v>
+        <v>186</v>
       </c>
       <c r="I26">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J26" t="s">
         <v>141</v>
       </c>
       <c r="K26">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="L26">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M26" t="s">
         <v>173</v>
       </c>
       <c r="N26">
-        <v>106</v>
+        <v>142</v>
       </c>
       <c r="O26">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P26" t="s">
         <v>205</v>
       </c>
       <c r="Q26">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R26">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S26" t="s">
         <v>237</v>
       </c>
       <c r="T26">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U26">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:21">
@@ -2807,64 +2807,64 @@
         <v>46</v>
       </c>
       <c r="B27">
-        <v>466</v>
+        <v>637</v>
       </c>
       <c r="C27">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="D27" t="s">
         <v>78</v>
       </c>
       <c r="E27">
-        <v>346</v>
+        <v>472</v>
       </c>
       <c r="F27">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="G27" t="s">
         <v>110</v>
       </c>
       <c r="H27">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="I27">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J27" t="s">
         <v>142</v>
       </c>
       <c r="K27">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="L27">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M27" t="s">
         <v>174</v>
       </c>
       <c r="N27">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="O27">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P27" t="s">
         <v>206</v>
       </c>
       <c r="Q27">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R27">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S27" t="s">
         <v>238</v>
       </c>
       <c r="T27">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U27">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -2872,64 +2872,64 @@
         <v>47</v>
       </c>
       <c r="B28">
-        <v>410</v>
+        <v>560</v>
       </c>
       <c r="C28">
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="D28" t="s">
         <v>79</v>
       </c>
       <c r="E28">
-        <v>378</v>
+        <v>516</v>
       </c>
       <c r="F28">
-        <v>257</v>
+        <v>335</v>
       </c>
       <c r="G28" t="s">
         <v>111</v>
       </c>
       <c r="H28">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="I28">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J28" t="s">
         <v>143</v>
       </c>
       <c r="K28">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="L28">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M28" t="s">
         <v>175</v>
       </c>
       <c r="N28">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="O28">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P28" t="s">
         <v>207</v>
       </c>
       <c r="Q28">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R28">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S28" t="s">
         <v>239</v>
       </c>
       <c r="T28">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U28">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:21">
@@ -2937,64 +2937,64 @@
         <v>48</v>
       </c>
       <c r="B29">
-        <v>490</v>
+        <v>670</v>
       </c>
       <c r="C29">
-        <v>390</v>
+        <v>510</v>
       </c>
       <c r="D29" t="s">
         <v>80</v>
       </c>
       <c r="E29">
-        <v>442</v>
+        <v>604</v>
       </c>
       <c r="F29">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="G29" t="s">
         <v>112</v>
       </c>
       <c r="H29">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="I29">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J29" t="s">
         <v>144</v>
       </c>
       <c r="K29">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="L29">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M29" t="s">
         <v>176</v>
       </c>
       <c r="N29">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="O29">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P29" t="s">
         <v>208</v>
       </c>
       <c r="Q29">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R29">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S29" t="s">
         <v>240</v>
       </c>
       <c r="T29">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U29">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:21">
@@ -3002,64 +3002,64 @@
         <v>49</v>
       </c>
       <c r="B30">
-        <v>354</v>
+        <v>483</v>
       </c>
       <c r="C30">
-        <v>409</v>
+        <v>535</v>
       </c>
       <c r="D30" t="s">
         <v>81</v>
       </c>
       <c r="E30">
-        <v>410</v>
+        <v>560</v>
       </c>
       <c r="F30">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="G30" t="s">
         <v>113</v>
       </c>
       <c r="H30">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="I30">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J30" t="s">
         <v>145</v>
       </c>
       <c r="K30">
-        <v>146</v>
+        <v>197</v>
       </c>
       <c r="L30">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M30" t="s">
         <v>177</v>
       </c>
       <c r="N30">
-        <v>146</v>
+        <v>197</v>
       </c>
       <c r="O30">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P30" t="s">
         <v>209</v>
       </c>
       <c r="Q30">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R30">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S30" t="s">
         <v>241</v>
       </c>
       <c r="T30">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U30">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -3067,64 +3067,64 @@
         <v>50</v>
       </c>
       <c r="B31">
-        <v>306</v>
+        <v>417</v>
       </c>
       <c r="C31">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="D31" t="s">
         <v>82</v>
       </c>
       <c r="E31">
-        <v>346</v>
+        <v>472</v>
       </c>
       <c r="F31">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="G31" t="s">
         <v>114</v>
       </c>
       <c r="H31">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I31">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J31" t="s">
         <v>146</v>
       </c>
       <c r="K31">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="L31">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M31" t="s">
         <v>178</v>
       </c>
       <c r="N31">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="O31">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P31" t="s">
         <v>210</v>
       </c>
       <c r="Q31">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R31">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S31" t="s">
         <v>242</v>
       </c>
       <c r="T31">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U31">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:21">
@@ -3132,64 +3132,64 @@
         <v>51</v>
       </c>
       <c r="B32">
-        <v>394</v>
+        <v>538</v>
       </c>
       <c r="C32">
-        <v>181</v>
+        <v>235</v>
       </c>
       <c r="D32" t="s">
         <v>83</v>
       </c>
       <c r="E32">
-        <v>362</v>
+        <v>494</v>
       </c>
       <c r="F32">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="G32" t="s">
         <v>115</v>
       </c>
       <c r="H32">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I32">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J32" t="s">
         <v>147</v>
       </c>
       <c r="K32">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L32">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M32" t="s">
         <v>179</v>
       </c>
       <c r="N32">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="O32">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P32" t="s">
         <v>211</v>
       </c>
       <c r="Q32">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R32">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S32" t="s">
         <v>243</v>
       </c>
       <c r="T32">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U32">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:21">
@@ -3197,64 +3197,64 @@
         <v>52</v>
       </c>
       <c r="B33">
-        <v>458</v>
+        <v>626</v>
       </c>
       <c r="C33">
-        <v>390</v>
+        <v>510</v>
       </c>
       <c r="D33" t="s">
         <v>84</v>
       </c>
       <c r="E33">
-        <v>418</v>
+        <v>571</v>
       </c>
       <c r="F33">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="G33" t="s">
         <v>116</v>
       </c>
       <c r="H33">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I33">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J33" t="s">
         <v>148</v>
       </c>
       <c r="K33">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="L33">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M33" t="s">
         <v>180</v>
       </c>
       <c r="N33">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="O33">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P33" t="s">
         <v>212</v>
       </c>
       <c r="Q33">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R33">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="S33" t="s">
         <v>244</v>
       </c>
       <c r="T33">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="U33">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated images and gitignore
</commit_message>
<xml_diff>
--- a/Study/conditions.xlsx
+++ b/Study/conditions.xlsx
@@ -1247,7 +1247,7 @@
         <v>22</v>
       </c>
       <c r="B3">
-        <v>571</v>
+        <v>593</v>
       </c>
       <c r="C3">
         <v>310</v>
@@ -1312,7 +1312,7 @@
         <v>23</v>
       </c>
       <c r="B4">
-        <v>901</v>
+        <v>923</v>
       </c>
       <c r="C4">
         <v>385</v>
@@ -1702,7 +1702,7 @@
         <v>29</v>
       </c>
       <c r="B10">
-        <v>615</v>
+        <v>648</v>
       </c>
       <c r="C10">
         <v>435</v>
@@ -2027,7 +2027,7 @@
         <v>34</v>
       </c>
       <c r="B15">
-        <v>582</v>
+        <v>615</v>
       </c>
       <c r="C15">
         <v>385</v>
@@ -2036,7 +2036,7 @@
         <v>66</v>
       </c>
       <c r="E15">
-        <v>483</v>
+        <v>494</v>
       </c>
       <c r="F15">
         <v>185</v>
@@ -2166,7 +2166,7 @@
         <v>68</v>
       </c>
       <c r="E17">
-        <v>472</v>
+        <v>494</v>
       </c>
       <c r="F17">
         <v>110</v>
@@ -2287,7 +2287,7 @@
         <v>38</v>
       </c>
       <c r="B19">
-        <v>483</v>
+        <v>857</v>
       </c>
       <c r="C19">
         <v>210</v>
@@ -2296,7 +2296,7 @@
         <v>70</v>
       </c>
       <c r="E19">
-        <v>472</v>
+        <v>494</v>
       </c>
       <c r="F19">
         <v>135</v>
@@ -2491,7 +2491,7 @@
         <v>73</v>
       </c>
       <c r="E22">
-        <v>472</v>
+        <v>494</v>
       </c>
       <c r="F22">
         <v>160</v>
@@ -2547,7 +2547,7 @@
         <v>42</v>
       </c>
       <c r="B23">
-        <v>626</v>
+        <v>648</v>
       </c>
       <c r="C23">
         <v>410</v>
@@ -2686,7 +2686,7 @@
         <v>76</v>
       </c>
       <c r="E25">
-        <v>472</v>
+        <v>494</v>
       </c>
       <c r="F25">
         <v>85</v>
@@ -2816,7 +2816,7 @@
         <v>78</v>
       </c>
       <c r="E27">
-        <v>472</v>
+        <v>494</v>
       </c>
       <c r="F27">
         <v>185</v>
@@ -3076,7 +3076,7 @@
         <v>82</v>
       </c>
       <c r="E31">
-        <v>472</v>
+        <v>494</v>
       </c>
       <c r="F31">
         <v>85</v>

</xml_diff>